<commit_message>
CHANGES ON 17TH JAN
INTEGRATING THE GRAPHS
</commit_message>
<xml_diff>
--- a/POCs/dailyat.xlsx
+++ b/POCs/dailyat.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781DACE2-A385-4595-9659-3CD13697CAD3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A8AA29-D8B9-4FD8-A147-9511EBDEA7D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="26">
   <si>
     <t>IN_TIME</t>
   </si>
@@ -28,9 +28,6 @@
     <t>OUT_TIME</t>
   </si>
   <si>
-    <t>HOURDIFF</t>
-  </si>
-  <si>
     <t>TIMESTAMP</t>
   </si>
   <si>
@@ -95,6 +92,12 @@
   </si>
   <si>
     <t>28/02/2018</t>
+  </si>
+  <si>
+    <t>SYSTEM</t>
+  </si>
+  <si>
+    <t>NOBEL</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,10 +504,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -513,18 +516,18 @@
         <v>1</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>0.30208333333333331</v>
@@ -532,8 +535,8 @@
       <c r="D2" s="3">
         <v>0.7895833333333333</v>
       </c>
-      <c r="E2" s="3">
-        <v>0.4458333333333333</v>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <v>43102</v>
@@ -541,10 +544,10 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
         <v>0.30555555555555552</v>
@@ -552,8 +555,8 @@
       <c r="D3" s="3">
         <v>0.84027777777777779</v>
       </c>
-      <c r="E3" s="3">
-        <v>0.49305555555555558</v>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F3" s="1">
         <v>43133</v>
@@ -561,10 +564,10 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3">
         <v>0.26319444444444445</v>
@@ -572,8 +575,8 @@
       <c r="D4" s="3">
         <v>0.55486111111111114</v>
       </c>
-      <c r="E4" s="3">
-        <v>0.25</v>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F4" s="1">
         <v>43161</v>
@@ -581,24 +584,26 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F5" s="1">
         <v>43192</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>0.30555555555555552</v>
@@ -606,8 +611,8 @@
       <c r="D6" s="3">
         <v>0.7416666666666667</v>
       </c>
-      <c r="E6" s="3">
-        <v>0.39444444444444443</v>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="1">
         <v>43222</v>
@@ -615,10 +620,10 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
         <v>0.29791666666666666</v>
@@ -626,8 +631,8 @@
       <c r="D7" s="3">
         <v>0.7993055555555556</v>
       </c>
-      <c r="E7" s="3">
-        <v>0.4597222222222222</v>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F7" s="1">
         <v>43253</v>
@@ -635,10 +640,10 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3">
         <v>0.30416666666666664</v>
@@ -646,8 +651,8 @@
       <c r="D8" s="3">
         <v>0.78125</v>
       </c>
-      <c r="E8" s="3">
-        <v>0.43541666666666662</v>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>43283</v>
@@ -655,10 +660,10 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3">
         <v>0.30833333333333335</v>
@@ -666,8 +671,8 @@
       <c r="D9" s="3">
         <v>0.77430555555555547</v>
       </c>
-      <c r="E9" s="3">
-        <v>0.42430555555555555</v>
+      <c r="E9" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="1">
         <v>43314</v>
@@ -675,10 +680,10 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3">
         <v>0.30763888888888891</v>
@@ -686,8 +691,8 @@
       <c r="D10" s="3">
         <v>0.7284722222222223</v>
       </c>
-      <c r="E10" s="3">
-        <v>0.37916666666666665</v>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F10" s="1">
         <v>43345</v>
@@ -695,10 +700,10 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3">
         <v>0.30833333333333335</v>
@@ -706,8 +711,8 @@
       <c r="D11" s="3">
         <v>0.7944444444444444</v>
       </c>
-      <c r="E11" s="3">
-        <v>0.24305555555555555</v>
+      <c r="E11" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F11" s="1">
         <v>43375</v>
@@ -715,10 +720,10 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
         <v>0.50069444444444444</v>
@@ -726,8 +731,8 @@
       <c r="D12" s="3">
         <v>0.78541666666666676</v>
       </c>
-      <c r="E12" s="3">
-        <v>0.44444444444444442</v>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F12" s="1">
         <v>43376</v>
@@ -735,10 +740,10 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3">
         <v>0.30763888888888891</v>
@@ -746,8 +751,8 @@
       <c r="D13" s="3">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E13" s="3">
-        <v>0.44236111111111115</v>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F13" s="1">
         <v>43436</v>
@@ -755,10 +760,10 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3">
         <v>0.34236111111111112</v>
@@ -766,19 +771,19 @@
       <c r="D14" s="3">
         <v>0.79027777777777775</v>
       </c>
-      <c r="E14" s="3">
-        <v>0.40625</v>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3">
         <v>0.30902777777777779</v>
@@ -786,75 +791,83 @@
       <c r="D15" s="3">
         <v>0.78472222222222221</v>
       </c>
-      <c r="E15" s="3">
-        <v>0.43402777777777773</v>
+      <c r="E15" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="3">
         <v>0.30486111111111108</v>
@@ -862,19 +875,19 @@
       <c r="D20" s="3">
         <v>0.69444444444444453</v>
       </c>
-      <c r="E20" s="3">
-        <v>0.34791666666666665</v>
+      <c r="E20" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="3">
         <v>0.30138888888888887</v>
@@ -882,19 +895,19 @@
       <c r="D21" s="3">
         <v>0.73125000000000007</v>
       </c>
-      <c r="E21" s="3">
-        <v>0.38819444444444445</v>
+      <c r="E21" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="3">
         <v>0.30416666666666664</v>
@@ -902,19 +915,19 @@
       <c r="D22" s="3">
         <v>0.81458333333333333</v>
       </c>
-      <c r="E22" s="3">
-        <v>0.46875</v>
+      <c r="E22" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3">
         <v>0.30277777777777776</v>
@@ -922,19 +935,19 @@
       <c r="D23" s="3">
         <v>0.77222222222222225</v>
       </c>
-      <c r="E23" s="3">
-        <v>0.42777777777777781</v>
+      <c r="E23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="3">
         <v>0.30208333333333331</v>
@@ -942,19 +955,19 @@
       <c r="D24" s="3">
         <v>0.72638888888888886</v>
       </c>
-      <c r="E24" s="3">
-        <v>0.38263888888888892</v>
+      <c r="E24" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="3">
         <v>0.30972222222222223</v>
@@ -962,19 +975,19 @@
       <c r="D25" s="3">
         <v>0.69027777777777777</v>
       </c>
-      <c r="E25" s="3">
-        <v>0.33888888888888885</v>
+      <c r="E25" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="3">
         <v>0.30486111111111108</v>
@@ -982,19 +995,19 @@
       <c r="D26" s="3">
         <v>0.69166666666666676</v>
       </c>
-      <c r="E26" s="3">
-        <v>0.34513888888888888</v>
+      <c r="E26" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="3">
         <v>0.30416666666666664</v>
@@ -1002,19 +1015,19 @@
       <c r="D27" s="3">
         <v>0.69305555555555554</v>
       </c>
-      <c r="E27" s="3">
-        <v>0.34722222222222227</v>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="3">
         <v>0.30277777777777776</v>
@@ -1022,19 +1035,19 @@
       <c r="D28" s="3">
         <v>0.7319444444444444</v>
       </c>
-      <c r="E28" s="3">
-        <v>0.38750000000000001</v>
+      <c r="E28" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="5">
         <v>0.29791666666666666</v>
@@ -1042,19 +1055,19 @@
       <c r="D29" s="5">
         <v>0.75624999999999998</v>
       </c>
-      <c r="E29" s="5">
-        <v>0.41666666666666669</v>
+      <c r="E29" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="3">
         <v>1.3194444444444444E-2</v>
@@ -1062,8 +1075,8 @@
       <c r="D30" s="3">
         <v>0.96597222222222223</v>
       </c>
-      <c r="E30" s="3">
-        <v>0.91111111111111109</v>
+      <c r="E30" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F30" s="1">
         <v>43102</v>
@@ -1071,10 +1084,10 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" s="3">
         <v>3.6111111111111115E-2</v>
@@ -1082,8 +1095,8 @@
       <c r="D31" s="3">
         <v>0.95416666666666661</v>
       </c>
-      <c r="E31" s="3">
-        <v>0.87638888888888899</v>
+      <c r="E31" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F31" s="1">
         <v>43133</v>
@@ -1091,10 +1104,10 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="3">
         <v>0.98749999999999993</v>
@@ -1102,8 +1115,8 @@
       <c r="D32" s="3">
         <v>0.9902777777777777</v>
       </c>
-      <c r="E32" s="3">
-        <v>2.7777777777777779E-3</v>
+      <c r="E32" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F32" s="1">
         <v>43161</v>
@@ -1111,10 +1124,10 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="3">
         <v>0.60069444444444442</v>
@@ -1122,8 +1135,8 @@
       <c r="D33" s="3">
         <v>0.94305555555555554</v>
       </c>
-      <c r="E33" s="3">
-        <v>0.30069444444444443</v>
+      <c r="E33" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F33" s="1">
         <v>43192</v>
@@ -1131,10 +1144,10 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" s="3">
         <v>0.9902777777777777</v>
@@ -1142,8 +1155,8 @@
       <c r="D34" s="3">
         <v>0.97361111111111109</v>
       </c>
-      <c r="E34" s="3">
-        <v>0.94166666666666676</v>
+      <c r="E34" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F34" s="1">
         <v>43222</v>
@@ -1151,10 +1164,10 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3">
         <v>1.1805555555555555E-2</v>
@@ -1162,8 +1175,8 @@
       <c r="D35" s="3">
         <v>0.11597222222222221</v>
       </c>
-      <c r="E35" s="3">
-        <v>0.10416666666666667</v>
+      <c r="E35" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F35" s="1">
         <v>43253</v>
@@ -1171,10 +1184,10 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="3">
         <v>0.63888888888888895</v>
@@ -1182,8 +1195,8 @@
       <c r="D36" s="3">
         <v>0.94791666666666663</v>
       </c>
-      <c r="E36" s="3">
-        <v>0.30902777777777779</v>
+      <c r="E36" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F36" s="1">
         <v>43283</v>
@@ -1191,10 +1204,10 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="3">
         <v>0.98125000000000007</v>
@@ -1202,8 +1215,8 @@
       <c r="D37" s="3">
         <v>0.99930555555555556</v>
       </c>
-      <c r="E37" s="3">
-        <v>0.97638888888888886</v>
+      <c r="E37" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F37" s="1">
         <v>43314</v>
@@ -1211,10 +1224,10 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="3">
         <v>3.472222222222222E-3</v>
@@ -1222,8 +1235,8 @@
       <c r="D38" s="3">
         <v>0.90277777777777779</v>
       </c>
-      <c r="E38" s="3">
-        <v>0.85763888888888884</v>
+      <c r="E38" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F38" s="1">
         <v>43345</v>
@@ -1231,10 +1244,10 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" s="3">
         <v>0.99583333333333324</v>
@@ -1242,8 +1255,8 @@
       <c r="D39" s="3">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E39" s="3">
-        <v>2.4999999999999998E-2</v>
+      <c r="E39" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F39" s="1">
         <v>43375</v>
@@ -1251,10 +1264,10 @@
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="3">
         <v>0.59444444444444444</v>
@@ -1262,8 +1275,8 @@
       <c r="D40" s="3">
         <v>0.90625</v>
       </c>
-      <c r="E40" s="3">
-        <v>0.27013888888888887</v>
+      <c r="E40" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F40" s="1">
         <v>43406</v>
@@ -1271,10 +1284,10 @@
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" s="3">
         <v>0.98333333333333339</v>
@@ -1282,8 +1295,8 @@
       <c r="D41" s="3">
         <v>0.91875000000000007</v>
       </c>
-      <c r="E41" s="3">
-        <v>0.89374999999999993</v>
+      <c r="E41" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F41" s="1">
         <v>43436</v>
@@ -1291,10 +1304,10 @@
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42" s="3">
         <v>1.7361111111111112E-2</v>
@@ -1302,19 +1315,19 @@
       <c r="D42" s="3">
         <v>0.9590277777777777</v>
       </c>
-      <c r="E42" s="3">
-        <v>0.9</v>
+      <c r="E42" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" s="3">
         <v>0.99652777777777779</v>
@@ -1322,19 +1335,19 @@
       <c r="D43" s="3">
         <v>0.88958333333333339</v>
       </c>
-      <c r="E43" s="3">
-        <v>0.85138888888888886</v>
+      <c r="E43" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" s="3">
         <v>0.99861111111111101</v>
@@ -1342,19 +1355,19 @@
       <c r="D44" s="3">
         <v>0.88402777777777775</v>
       </c>
-      <c r="E44" s="3">
-        <v>0.84375</v>
+      <c r="E44" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" s="3">
         <v>0.97986111111111107</v>
@@ -1362,19 +1375,19 @@
       <c r="D45" s="3">
         <v>0.9590277777777777</v>
       </c>
-      <c r="E45" s="3">
-        <v>0.9375</v>
+      <c r="E45" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46" s="3">
         <v>0.9868055555555556</v>
@@ -1382,19 +1395,19 @@
       <c r="D46" s="3">
         <v>0.98819444444444438</v>
       </c>
-      <c r="E46" s="3">
-        <v>1.3888888888888889E-3</v>
+      <c r="E46" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47" s="3">
         <v>0.62152777777777779</v>
@@ -1402,19 +1415,19 @@
       <c r="D47" s="3">
         <v>0.86736111111111114</v>
       </c>
-      <c r="E47" s="3">
-        <v>0.20416666666666669</v>
+      <c r="E47" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="3">
         <v>5.5555555555555558E-3</v>
@@ -1422,19 +1435,19 @@
       <c r="D48" s="3">
         <v>0.87222222222222223</v>
       </c>
-      <c r="E48" s="3">
-        <v>0.82500000000000007</v>
+      <c r="E48" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" s="3">
         <v>1.1805555555555555E-2</v>
@@ -1442,19 +1455,19 @@
       <c r="D49" s="3">
         <v>0.90625</v>
       </c>
-      <c r="E49" s="3">
-        <v>0.85277777777777775</v>
+      <c r="E49" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C50" s="3">
         <v>0.9916666666666667</v>
@@ -1462,19 +1475,19 @@
       <c r="D50" s="3">
         <v>0.97569444444444453</v>
       </c>
-      <c r="E50" s="3">
-        <v>0.94236111111111109</v>
+      <c r="E50" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C51" s="3">
         <v>3.4027777777777775E-2</v>
@@ -1482,19 +1495,19 @@
       <c r="D51" s="3">
         <v>0.9472222222222223</v>
       </c>
-      <c r="E51" s="3">
-        <v>0.87152777777777779</v>
+      <c r="E51" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52" s="3">
         <v>1.7361111111111112E-2</v>
@@ -1502,19 +1515,19 @@
       <c r="D52" s="3">
         <v>0.92152777777777783</v>
       </c>
-      <c r="E52" s="3">
-        <v>0.86249999999999993</v>
+      <c r="E52" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" s="3">
         <v>1.3888888888888889E-3</v>
@@ -1522,19 +1535,19 @@
       <c r="D53" s="3">
         <v>2.2222222222222223E-2</v>
       </c>
-      <c r="E53" s="3">
-        <v>2.0833333333333332E-2</v>
+      <c r="E53" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54" s="3">
         <v>0.63750000000000007</v>
@@ -1542,19 +1555,19 @@
       <c r="D54" s="3">
         <v>0.97569444444444453</v>
       </c>
-      <c r="E54" s="3">
-        <v>0.29652777777777778</v>
+      <c r="E54" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" s="3">
         <v>0.97986111111111107</v>
@@ -1562,33 +1575,35 @@
       <c r="D55" s="3">
         <v>0.12361111111111112</v>
       </c>
-      <c r="E55" s="3">
-        <v>0.14375000000000002</v>
+      <c r="E55" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
+      <c r="E56" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F56" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57" s="5">
         <v>0.63888888888888895</v>
@@ -1596,12 +1611,24 @@
       <c r="D57" s="5">
         <v>0.95416666666666661</v>
       </c>
-      <c r="E57" s="5">
-        <v>0.31527777777777777</v>
+      <c r="E57" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>